<commit_message>
modify map for clustering
</commit_message>
<xml_diff>
--- a/ressources/people_location.xlsx
+++ b/ressources/people_location.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JSA\Documents\LABERCA\W4M\workflow4metabolomics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JSA\Documents\LABERCA\W4M\workflow4metabolomics\ressources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="80">
   <si>
     <t>people</t>
   </si>
@@ -41,9 +41,6 @@
     <t>country</t>
   </si>
   <si>
-    <t>lon</t>
-  </si>
-  <si>
     <t>lat</t>
   </si>
   <si>
@@ -99,13 +96,181 @@
   </si>
   <si>
     <t>48.72680</t>
+  </si>
+  <si>
+    <t>long</t>
+  </si>
+  <si>
+    <t>Binta Diémé</t>
+  </si>
+  <si>
+    <t>Charlotte Joly</t>
+  </si>
+  <si>
+    <t>Christophe Duperier</t>
+  </si>
+  <si>
+    <t>Cécile Canlet</t>
+  </si>
+  <si>
+    <t>Cédric Delporte</t>
+  </si>
+  <si>
+    <t>Céline Dalle</t>
+  </si>
+  <si>
+    <t>David Benaben</t>
+  </si>
+  <si>
+    <t>Eric Venot</t>
+  </si>
+  <si>
+    <t>Etienne Thévenot</t>
+  </si>
+  <si>
+    <t>Florence Soulard</t>
+  </si>
+  <si>
+    <t>Franck Gacomoni</t>
+  </si>
+  <si>
+    <t>Isabelle Schmitz</t>
+  </si>
+  <si>
+    <t>Marie Tremblay-Franco</t>
+  </si>
+  <si>
+    <t>Mélanie Pétéra</t>
+  </si>
+  <si>
+    <t>Nils Paulhe</t>
+  </si>
+  <si>
+    <t>Ralf Weber</t>
+  </si>
+  <si>
+    <t>Sylvain Chéreau</t>
+  </si>
+  <si>
+    <t>Sylvain Dechaumet</t>
+  </si>
+  <si>
+    <t>Belgique</t>
+  </si>
+  <si>
+    <t>United-Kingdom</t>
+  </si>
+  <si>
+    <t>26 Av. Léon Blum</t>
+  </si>
+  <si>
+    <t>Clermont-Ferrand</t>
+  </si>
+  <si>
+    <t>45.7717170715332</t>
+  </si>
+  <si>
+    <t>3.0734329223632812</t>
+  </si>
+  <si>
+    <t>IGEPP</t>
+  </si>
+  <si>
+    <t>PFEM</t>
+  </si>
+  <si>
+    <t>TOXALIM</t>
+  </si>
+  <si>
+    <t>180 chemin de Tournefeuille</t>
+  </si>
+  <si>
+    <t>Toulouse</t>
+  </si>
+  <si>
+    <t>43.59865188598633</t>
+  </si>
+  <si>
+    <t>1.3715448379516602</t>
+  </si>
+  <si>
+    <t>ULB</t>
+  </si>
+  <si>
+    <t>Boulevard de Triomphe, access 2</t>
+  </si>
+  <si>
+    <t>Brussels</t>
+  </si>
+  <si>
+    <t>50.818092092542436</t>
+  </si>
+  <si>
+    <t>4.3961032004916145</t>
+  </si>
+  <si>
+    <t>IRBA</t>
+  </si>
+  <si>
+    <t>MTS</t>
+  </si>
+  <si>
+    <t>ABiMS</t>
+  </si>
+  <si>
+    <t>Helge Hecht</t>
+  </si>
+  <si>
+    <t>RECETOX</t>
+  </si>
+  <si>
+    <t>Brétigny-sur-Orge</t>
+  </si>
+  <si>
+    <t>1 place du Général Valérie André</t>
+  </si>
+  <si>
+    <t>48.604610443115234</t>
+  </si>
+  <si>
+    <t>2.3223390579223633</t>
+  </si>
+  <si>
+    <t>BFP</t>
+  </si>
+  <si>
+    <t>71, avenue Edouard Bourlaux</t>
+  </si>
+  <si>
+    <t>Villenave d’Ornon</t>
+  </si>
+  <si>
+    <t>44.786312103271484</t>
+  </si>
+  <si>
+    <t>-0.5724135637283325</t>
+  </si>
+  <si>
+    <t>GABI</t>
+  </si>
+  <si>
+    <t>Domaine de Vilvert</t>
+  </si>
+  <si>
+    <t>Jouy-en-josas</t>
+  </si>
+  <si>
+    <t>2.1767607</t>
+  </si>
+  <si>
+    <t>48.765236</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,6 +281,25 @@
     <font>
       <sz val="8"/>
       <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF040404"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -140,10 +324,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,122 +613,506 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2">
+        <v>63000</v>
+      </c>
+      <c r="G2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3">
+        <v>63000</v>
+      </c>
+      <c r="G3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4">
+        <v>63000</v>
+      </c>
+      <c r="G4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" s="3">
+        <v>31027</v>
+      </c>
+      <c r="G5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F6" s="4">
+        <v>1050</v>
+      </c>
+      <c r="G6" t="s">
+        <v>58</v>
+      </c>
+      <c r="H6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" t="s">
+        <v>67</v>
+      </c>
+      <c r="F7">
+        <v>91220</v>
+      </c>
+      <c r="G7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" t="s">
+        <v>71</v>
+      </c>
+      <c r="F8">
+        <v>33140</v>
+      </c>
+      <c r="G8" t="s">
+        <v>72</v>
+      </c>
+      <c r="H8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" t="s">
+        <v>75</v>
+      </c>
+      <c r="E9" t="s">
+        <v>76</v>
+      </c>
+      <c r="F9">
+        <v>78350</v>
+      </c>
+      <c r="G9" t="s">
+        <v>77</v>
+      </c>
+      <c r="H9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" t="s">
+        <v>62</v>
+      </c>
+      <c r="H10" t="s">
+        <v>13</v>
+      </c>
+      <c r="K10" s="5"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11" s="4">
+        <v>1050</v>
+      </c>
+      <c r="G11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12">
+        <v>63000</v>
+      </c>
+      <c r="G12" t="s">
+        <v>46</v>
+      </c>
+      <c r="H12" t="s">
+        <v>13</v>
+      </c>
+      <c r="K12" s="5"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" t="s">
         <v>18</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="D13" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13">
+        <v>58965</v>
+      </c>
+      <c r="G13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C14" t="s">
+        <v>36</v>
+      </c>
+      <c r="H14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15">
+        <v>44307</v>
+      </c>
+      <c r="G15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C16" t="s">
+        <v>37</v>
+      </c>
+      <c r="H16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" t="s">
+        <v>45</v>
+      </c>
+      <c r="F17">
+        <v>63000</v>
+      </c>
+      <c r="G17" t="s">
+        <v>46</v>
+      </c>
+      <c r="H17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" t="s">
+        <v>45</v>
+      </c>
+      <c r="F18">
+        <v>63000</v>
+      </c>
+      <c r="G18" t="s">
+        <v>46</v>
+      </c>
+      <c r="H18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C19" t="s">
+        <v>40</v>
+      </c>
+      <c r="H19" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C20" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" t="s">
+        <v>49</v>
+      </c>
+      <c r="H20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C21" t="s">
+        <v>42</v>
+      </c>
+      <c r="H21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="D22" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="F22">
+        <v>44307</v>
+      </c>
+      <c r="G22" t="s">
         <v>8</v>
       </c>
-      <c r="D2">
-        <v>44307</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="H22" t="s">
         <v>9</v>
       </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3">
-        <v>44307</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4">
-        <v>58965</v>
-      </c>
-      <c r="E4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H5" s="2"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C23" t="s">
+        <v>64</v>
+      </c>
+      <c r="D23" t="s">
+        <v>65</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
modify names for link from map
</commit_message>
<xml_diff>
--- a/ressources/people_location.xlsx
+++ b/ressources/people_location.xlsx
@@ -128,12 +128,6 @@
     <t>Etienne Thévenot</t>
   </si>
   <si>
-    <t>Florence Soulard</t>
-  </si>
-  <si>
-    <t>Franck Gacomoni</t>
-  </si>
-  <si>
     <t>Isabelle Schmitz</t>
   </si>
   <si>
@@ -342,6 +336,12 @@
   </si>
   <si>
     <t>MUNI Campus in building A29</t>
+  </si>
+  <si>
+    <t>Florence Souard</t>
+  </si>
+  <si>
+    <t>Franck Giacomoni</t>
   </si>
 </sst>
 </file>
@@ -702,7 +702,7 @@
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -745,25 +745,25 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C2" t="s">
         <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F2">
         <v>63000</v>
       </c>
       <c r="G2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H2" t="s">
         <v>13</v>
@@ -771,25 +771,25 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C3" t="s">
         <v>26</v>
       </c>
       <c r="D3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F3">
         <v>63000</v>
       </c>
       <c r="G3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H3" t="s">
         <v>13</v>
@@ -797,10 +797,10 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C4" t="s">
         <v>27</v>
@@ -809,13 +809,13 @@
         <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F4">
         <v>63000</v>
       </c>
       <c r="G4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H4" t="s">
         <v>13</v>
@@ -823,25 +823,25 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C5" t="s">
         <v>28</v>
       </c>
       <c r="D5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F5" s="3">
         <v>31027</v>
       </c>
       <c r="G5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H5" t="s">
         <v>13</v>
@@ -849,51 +849,51 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C6" t="s">
         <v>29</v>
       </c>
       <c r="D6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F6" s="4">
         <v>1050</v>
       </c>
       <c r="G6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C7" t="s">
         <v>30</v>
       </c>
       <c r="D7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F7">
         <v>91220</v>
       </c>
       <c r="G7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H7" t="s">
         <v>13</v>
@@ -901,25 +901,25 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C8" t="s">
         <v>31</v>
       </c>
       <c r="D8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F8">
         <v>33140</v>
       </c>
       <c r="G8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H8" t="s">
         <v>13</v>
@@ -927,25 +927,25 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C9" t="s">
         <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F9">
         <v>78350</v>
       </c>
       <c r="G9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H9" t="s">
         <v>13</v>
@@ -953,19 +953,19 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B10" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C10" t="s">
         <v>33</v>
       </c>
       <c r="D10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G10" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H10" t="s">
         <v>13</v>
@@ -974,51 +974,51 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>104</v>
       </c>
       <c r="D11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F11" s="4">
         <v>1050</v>
       </c>
       <c r="G11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" t="s">
+        <v>105</v>
+      </c>
+      <c r="D12" t="s">
         <v>48</v>
       </c>
-      <c r="B12" t="s">
-        <v>47</v>
-      </c>
-      <c r="C12" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" t="s">
-        <v>50</v>
-      </c>
       <c r="E12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F12">
         <v>63000</v>
       </c>
       <c r="G12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H12" t="s">
         <v>13</v>
@@ -1036,7 +1036,7 @@
         <v>18</v>
       </c>
       <c r="D13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E13" t="s">
         <v>20</v>
@@ -1053,25 +1053,25 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>82</v>
+      </c>
+      <c r="B14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" t="s">
+        <v>83</v>
+      </c>
+      <c r="E14" t="s">
         <v>84</v>
-      </c>
-      <c r="B14" t="s">
-        <v>83</v>
-      </c>
-      <c r="C14" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14" t="s">
-        <v>85</v>
-      </c>
-      <c r="E14" t="s">
-        <v>86</v>
       </c>
       <c r="F14">
         <v>76821</v>
       </c>
       <c r="G14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H14" t="s">
         <v>13</v>
@@ -1105,25 +1105,25 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B16" t="s">
+        <v>87</v>
+      </c>
+      <c r="C16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" t="s">
+        <v>86</v>
+      </c>
+      <c r="E16" t="s">
         <v>89</v>
-      </c>
-      <c r="C16" t="s">
-        <v>37</v>
-      </c>
-      <c r="D16" t="s">
-        <v>88</v>
-      </c>
-      <c r="E16" t="s">
-        <v>91</v>
       </c>
       <c r="F16">
         <v>31300</v>
       </c>
       <c r="G16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H16" t="s">
         <v>13</v>
@@ -1131,25 +1131,25 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" t="s">
         <v>48</v>
       </c>
-      <c r="B17" t="s">
-        <v>47</v>
-      </c>
-      <c r="C17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D17" t="s">
-        <v>50</v>
-      </c>
       <c r="E17" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F17">
         <v>63000</v>
       </c>
       <c r="G17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H17" t="s">
         <v>13</v>
@@ -1157,25 +1157,25 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" t="s">
         <v>48</v>
       </c>
-      <c r="B18" t="s">
-        <v>47</v>
-      </c>
-      <c r="C18" t="s">
-        <v>39</v>
-      </c>
-      <c r="D18" t="s">
-        <v>50</v>
-      </c>
       <c r="E18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F18">
         <v>63000</v>
       </c>
       <c r="G18" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H18" t="s">
         <v>13</v>
@@ -1183,51 +1183,51 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B19" t="s">
+        <v>90</v>
+      </c>
+      <c r="C19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" t="s">
+        <v>94</v>
+      </c>
+      <c r="E19" t="s">
+        <v>91</v>
+      </c>
+      <c r="F19" t="s">
         <v>92</v>
       </c>
-      <c r="C19" t="s">
-        <v>40</v>
-      </c>
-      <c r="D19" t="s">
-        <v>96</v>
-      </c>
-      <c r="E19" t="s">
+      <c r="G19" t="s">
         <v>93</v>
       </c>
-      <c r="F19" t="s">
-        <v>94</v>
-      </c>
-      <c r="G19" t="s">
-        <v>95</v>
-      </c>
       <c r="H19" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B20" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C20" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D20" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E20" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F20">
         <v>35650</v>
       </c>
       <c r="G20" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H20" t="s">
         <v>13</v>
@@ -1235,16 +1235,16 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B21" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C21" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D21" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H21" t="s">
         <v>13</v>
@@ -1278,22 +1278,22 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>101</v>
+      </c>
+      <c r="B23" t="s">
+        <v>100</v>
+      </c>
+      <c r="C23" t="s">
+        <v>61</v>
+      </c>
+      <c r="D23" t="s">
+        <v>62</v>
+      </c>
+      <c r="E23" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B23" t="s">
+      <c r="G23" t="s">
         <v>102</v>
-      </c>
-      <c r="C23" t="s">
-        <v>63</v>
-      </c>
-      <c r="D23" t="s">
-        <v>64</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="G23" t="s">
-        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
move christophe and helge
</commit_message>
<xml_diff>
--- a/ressources/people_location.xlsx
+++ b/ressources/people_location.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="98">
   <si>
     <t>people</t>
   </si>
@@ -83,9 +83,6 @@
     <t>Gildas LeCorguillé</t>
   </si>
   <si>
-    <t>INRAE</t>
-  </si>
-  <si>
     <t>Place Georges Tessier</t>
   </si>
   <si>
@@ -107,9 +104,6 @@
     <t>Charlotte Joly</t>
   </si>
   <si>
-    <t>Christophe Duperier</t>
-  </si>
-  <si>
     <t>Cécile Canlet</t>
   </si>
   <si>
@@ -209,12 +203,6 @@
     <t>ABiMS</t>
   </si>
   <si>
-    <t>Helge Hecht</t>
-  </si>
-  <si>
-    <t>RECETOX</t>
-  </si>
-  <si>
     <t>Brétigny-sur-Orge</t>
   </si>
   <si>
@@ -324,18 +312,6 @@
   </si>
   <si>
     <t>-1.9311562376160851</t>
-  </si>
-  <si>
-    <t>49.17647910080244</t>
-  </si>
-  <si>
-    <t>16.569918125482715</t>
-  </si>
-  <si>
-    <t>Brno-Bohunice, Kamenice 753/5,</t>
-  </si>
-  <si>
-    <t>MUNI Campus in building A29</t>
   </si>
   <si>
     <t>Florence Souard</t>
@@ -348,7 +324,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -381,13 +357,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -409,7 +378,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -418,7 +387,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -699,16 +667,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.21875" customWidth="1"/>
+    <col min="2" max="2" width="29.44140625" customWidth="1"/>
     <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.77734375" bestFit="1" customWidth="1"/>
@@ -719,7 +687,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
         <v>5</v>
@@ -745,25 +713,25 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
         <v>46</v>
       </c>
-      <c r="B2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" t="s">
-        <v>48</v>
-      </c>
       <c r="E2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F2">
         <v>63000</v>
       </c>
       <c r="G2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H2" t="s">
         <v>13</v>
@@ -771,51 +739,51 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
         <v>46</v>
       </c>
-      <c r="B3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" t="s">
-        <v>48</v>
-      </c>
       <c r="E3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F3">
         <v>63000</v>
       </c>
       <c r="G3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>46</v>
+      <c r="A4" t="s">
+        <v>51</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F4">
-        <v>63000</v>
+        <v>47</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" s="3">
+        <v>31027</v>
       </c>
       <c r="G4" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="H4" t="s">
         <v>13</v>
@@ -823,77 +791,77 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" t="s">
-        <v>49</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F5" s="3">
-        <v>31027</v>
+      <c r="F5" s="4">
+        <v>1050</v>
       </c>
       <c r="G5" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="H5" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
         <v>57</v>
       </c>
-      <c r="C6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" t="s">
-        <v>54</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="F6" s="4">
-        <v>1050</v>
+      <c r="E6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F6">
+        <v>91220</v>
       </c>
       <c r="G6" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="H6" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" t="s">
         <v>66</v>
       </c>
-      <c r="B7" t="s">
-        <v>65</v>
-      </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="E7" t="s">
         <v>64</v>
       </c>
       <c r="F7">
-        <v>91220</v>
+        <v>33140</v>
       </c>
       <c r="G7" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H7" t="s">
         <v>13</v>
@@ -904,22 +872,22 @@
         <v>71</v>
       </c>
       <c r="B8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" t="s">
+        <v>68</v>
+      </c>
+      <c r="E8" t="s">
+        <v>69</v>
+      </c>
+      <c r="F8">
+        <v>78350</v>
+      </c>
+      <c r="G8" t="s">
         <v>70</v>
-      </c>
-      <c r="C8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" t="s">
-        <v>67</v>
-      </c>
-      <c r="E8" t="s">
-        <v>68</v>
-      </c>
-      <c r="F8">
-        <v>33140</v>
-      </c>
-      <c r="G8" t="s">
-        <v>69</v>
       </c>
       <c r="H8" t="s">
         <v>13</v>
@@ -927,22 +895,16 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9" t="s">
         <v>75</v>
       </c>
-      <c r="B9" t="s">
-        <v>76</v>
-      </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D9" t="s">
-        <v>72</v>
-      </c>
-      <c r="E9" t="s">
         <v>73</v>
-      </c>
-      <c r="F9">
-        <v>78350</v>
       </c>
       <c r="G9" t="s">
         <v>74</v>
@@ -950,180 +912,186 @@
       <c r="H9" t="s">
         <v>13</v>
       </c>
+      <c r="K9" s="5"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
       <c r="B10" t="s">
-        <v>79</v>
+        <v>55</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>96</v>
       </c>
       <c r="D10" t="s">
-        <v>77</v>
+        <v>52</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10" s="4">
+        <v>1050</v>
       </c>
       <c r="G10" t="s">
-        <v>78</v>
+        <v>54</v>
       </c>
       <c r="H10" t="s">
-        <v>13</v>
-      </c>
-      <c r="K10" s="5"/>
+        <v>39</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>58</v>
+      <c r="A11" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="B11" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="C11" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="D11" t="s">
-        <v>54</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="F11" s="4">
-        <v>1050</v>
+        <v>46</v>
+      </c>
+      <c r="E11" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11">
+        <v>63000</v>
       </c>
       <c r="G11" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="H11" t="s">
-        <v>41</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="K11" s="5"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12">
+        <v>58965</v>
+      </c>
+      <c r="G12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>78</v>
+      </c>
+      <c r="B13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" t="s">
+        <v>79</v>
+      </c>
+      <c r="E13" t="s">
+        <v>80</v>
+      </c>
+      <c r="F13">
+        <v>76821</v>
+      </c>
+      <c r="G13" t="s">
+        <v>81</v>
+      </c>
+      <c r="H13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14">
+        <v>44307</v>
+      </c>
+      <c r="G14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>84</v>
+      </c>
+      <c r="B15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" t="s">
+        <v>82</v>
+      </c>
+      <c r="E15" t="s">
+        <v>85</v>
+      </c>
+      <c r="F15">
+        <v>31300</v>
+      </c>
+      <c r="G15" t="s">
+        <v>49</v>
+      </c>
+      <c r="H15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" t="s">
         <v>46</v>
       </c>
-      <c r="B12" t="s">
-        <v>45</v>
-      </c>
-      <c r="C12" t="s">
-        <v>105</v>
-      </c>
-      <c r="D12" t="s">
-        <v>48</v>
-      </c>
-      <c r="E12" t="s">
-        <v>43</v>
-      </c>
-      <c r="F12">
+      <c r="E16" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16">
         <v>63000</v>
       </c>
-      <c r="G12" t="s">
-        <v>44</v>
-      </c>
-      <c r="H12" t="s">
-        <v>13</v>
-      </c>
-      <c r="K12" s="5"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" t="s">
-        <v>60</v>
-      </c>
-      <c r="E13" t="s">
-        <v>20</v>
-      </c>
-      <c r="F13">
-        <v>58965</v>
-      </c>
-      <c r="G13" t="s">
-        <v>21</v>
-      </c>
-      <c r="H13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C14" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" t="s">
-        <v>83</v>
-      </c>
-      <c r="E14" t="s">
-        <v>84</v>
-      </c>
-      <c r="F14">
-        <v>76821</v>
-      </c>
-      <c r="G14" t="s">
-        <v>85</v>
-      </c>
-      <c r="H14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F15">
-        <v>44307</v>
-      </c>
-      <c r="G15" t="s">
-        <v>8</v>
-      </c>
-      <c r="H15" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>88</v>
-      </c>
-      <c r="B16" t="s">
-        <v>87</v>
-      </c>
-      <c r="C16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" t="s">
-        <v>86</v>
-      </c>
-      <c r="E16" t="s">
-        <v>89</v>
-      </c>
-      <c r="F16">
-        <v>31300</v>
-      </c>
       <c r="G16" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="H16" t="s">
         <v>13</v>
@@ -1131,169 +1099,123 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" t="s">
         <v>46</v>
       </c>
-      <c r="B17" t="s">
-        <v>45</v>
-      </c>
-      <c r="C17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D17" t="s">
-        <v>48</v>
-      </c>
       <c r="E17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F17">
         <v>63000</v>
       </c>
       <c r="G17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H17" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>46</v>
+      <c r="A18" t="s">
+        <v>95</v>
       </c>
       <c r="B18" t="s">
-        <v>45</v>
+        <v>86</v>
       </c>
       <c r="C18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D18" t="s">
-        <v>48</v>
+        <v>90</v>
       </c>
       <c r="E18" t="s">
-        <v>43</v>
-      </c>
-      <c r="F18">
-        <v>63000</v>
+        <v>87</v>
+      </c>
+      <c r="F18" t="s">
+        <v>88</v>
       </c>
       <c r="G18" t="s">
-        <v>44</v>
+        <v>89</v>
       </c>
       <c r="H18" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B19" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D19" t="s">
-        <v>94</v>
+        <v>45</v>
       </c>
       <c r="E19" t="s">
         <v>91</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19">
+        <v>35650</v>
+      </c>
+      <c r="G19" t="s">
         <v>92</v>
       </c>
-      <c r="G19" t="s">
-        <v>93</v>
-      </c>
       <c r="H19" t="s">
-        <v>42</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="B20" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
       <c r="C20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D20" t="s">
-        <v>47</v>
-      </c>
-      <c r="E20" t="s">
-        <v>95</v>
-      </c>
-      <c r="F20">
-        <v>35650</v>
-      </c>
-      <c r="G20" t="s">
-        <v>96</v>
+        <v>73</v>
       </c>
       <c r="H20" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>80</v>
+      <c r="A21" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="B21" t="s">
-        <v>79</v>
+        <v>10</v>
       </c>
       <c r="C21" t="s">
-        <v>40</v>
+        <v>6</v>
       </c>
       <c r="D21" t="s">
-        <v>77</v>
+        <v>16</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F21">
+        <v>44307</v>
+      </c>
+      <c r="G21" t="s">
+        <v>8</v>
       </c>
       <c r="H21" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B22" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" t="s">
-        <v>16</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F22">
-        <v>44307</v>
-      </c>
-      <c r="G22" t="s">
-        <v>8</v>
-      </c>
-      <c r="H22" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>101</v>
-      </c>
-      <c r="B23" t="s">
-        <v>100</v>
-      </c>
-      <c r="C23" t="s">
-        <v>61</v>
-      </c>
-      <c r="D23" t="s">
-        <v>62</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="G23" t="s">
-        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>